<commit_message>
various lookup tables to analyze ADA db content
</commit_message>
<xml_diff>
--- a/ADA-FileExtensions.xlsx
+++ b/ADA-FileExtensions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\.shortcut-targets-by-id\1pxYQnB_JBE8lYKR7m-VcgWZ9oyOJcQnc\AstroDB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944a82e2ddcde9eb/Documents/GithubC/smrgeoinfo/ada-metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0A3E6C-559D-445F-B1A2-7F3E2CEF4369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{CD0A3E6C-559D-445F-B1A2-7F3E2CEF4369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5278F8FD-E7D9-45C8-852C-228527120FB1}"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="3075" windowWidth="26685" windowHeight="15030" xr2:uid="{6B927432-2DD4-440C-AC82-B9813562449D}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="25965" windowHeight="14010" xr2:uid="{6B927432-2DD4-440C-AC82-B9813562449D}"/>
   </bookViews>
   <sheets>
     <sheet name="adaFileExtensions" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="141">
   <si>
     <t>id</t>
   </si>
@@ -323,9 +323,6 @@
     <t>Electron Microscopy Dataset</t>
   </si>
   <si>
-    <t xml:space="preserve"> HDF5-based interchange file format for electron microscopy data and metadata</t>
-  </si>
-  <si>
     <t>https://emdatasets.com/format/</t>
   </si>
   <si>
@@ -368,9 +365,6 @@
     <t>Spectral Data Exchange File</t>
   </si>
   <si>
-    <t>For astromat archive, these are only allowed as part of a shapefile composite dataset.</t>
-  </si>
-  <si>
     <t>.cdf</t>
   </si>
   <si>
@@ -405,6 +399,63 @@
   </si>
   <si>
     <t>https://www.adobe.com/creativecloud/file-types/video/container/m4v.html</t>
+  </si>
+  <si>
+    <t>image/bmp</t>
+  </si>
+  <si>
+    <t>Bitmap graphic</t>
+  </si>
+  <si>
+    <t>cpg</t>
+  </si>
+  <si>
+    <t>application/x-cpg</t>
+  </si>
+  <si>
+    <t>extension used for text and binary files, need to know the context to get the type either text/plain or application/octet-stream</t>
+  </si>
+  <si>
+    <t>application/x-dbf</t>
+  </si>
+  <si>
+    <t>For astromat archive, these are only allowed as part of a shapefile composite dataset.  Various mime type extensions are used</t>
+  </si>
+  <si>
+    <t>application/vnd.shp</t>
+  </si>
+  <si>
+    <t>application/vnd.shx</t>
+  </si>
+  <si>
+    <t>shape files are bundle with .shp, .shx, and .dbf</t>
+  </si>
+  <si>
+    <t>application/vnd.openxmlformats-officedocument.spreadsheetml.sheet</t>
+  </si>
+  <si>
+    <t>guess this is a plain text file</t>
+  </si>
+  <si>
+    <t>log file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The .exp extension is a proprietary format used by specific mass spectrometry software for exporting data. </t>
+  </si>
+  <si>
+    <t>application/octet-stream</t>
+  </si>
+  <si>
+    <t>mass spectrometry data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The TIFF format is flexible and is designed to store multiple images within a single file. When a program creates a "TIFF stack" or "TIFF movie," it's simply a TIFF file with multiple pages or image frames. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">required in MCICPMS raw data delivery. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> HDF5-based interchange file format for electron microscopy data and metadata; h5 dump will work with example I have</t>
   </si>
 </sst>
 </file>
@@ -897,9 +948,14 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -957,6 +1013,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1278,702 +1338,824 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D95B8BC-088D-4878-B6B7-898DD2B70A3D}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="3" max="3" width="29.5703125" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
-    <col min="5" max="5" width="56.5703125" customWidth="1"/>
+    <col min="4" max="4" width="34.85546875" customWidth="1"/>
+    <col min="5" max="5" width="55.7109375" customWidth="1"/>
+    <col min="6" max="6" width="49.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>34</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>35</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="C27" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>36</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>37</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>38</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>39</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>40</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>61</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>62</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>63</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>64</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>65</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>66</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+    </row>
+    <row r="39" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>1067</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>62</v>
-      </c>
-      <c r="B4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>63</v>
-      </c>
-      <c r="B6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>38</v>
-      </c>
-      <c r="B7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="F39" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>34</v>
-      </c>
-      <c r="B8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" t="s">
-        <v>95</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    </row>
+    <row r="40" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>1068</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C9" t="s">
-        <v>110</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="F40" s="1"/>
+    </row>
+    <row r="41" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>1069</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="275.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>1070</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F42" s="1"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>1071</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E43" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>1072</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>3</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>5</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>7</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>8</v>
-      </c>
-      <c r="B16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>61</v>
-      </c>
-      <c r="B17" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>18</v>
-      </c>
-      <c r="B18" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" t="s">
-        <v>51</v>
-      </c>
-      <c r="E19" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>39</v>
-      </c>
-      <c r="B20" t="s">
-        <v>71</v>
-      </c>
-      <c r="C20" t="s">
-        <v>121</v>
-      </c>
-      <c r="D20" t="s">
-        <v>119</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F20" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>16</v>
-      </c>
-      <c r="B21" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" t="s">
-        <v>122</v>
-      </c>
-      <c r="D21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>101</v>
-      </c>
-      <c r="C22" t="s">
-        <v>110</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="C44" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>2</v>
-      </c>
-      <c r="B23" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" t="s">
-        <v>89</v>
-      </c>
-      <c r="D23" t="s">
-        <v>90</v>
-      </c>
-      <c r="E23" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>37</v>
-      </c>
-      <c r="B24" t="s">
-        <v>69</v>
-      </c>
-      <c r="C24" t="s">
-        <v>89</v>
-      </c>
-      <c r="D24" t="s">
-        <v>90</v>
-      </c>
-      <c r="E24" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>10</v>
-      </c>
-      <c r="B25" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" t="s">
-        <v>98</v>
-      </c>
-      <c r="D25" t="s">
-        <v>24</v>
-      </c>
-      <c r="E25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>22</v>
-      </c>
-      <c r="B26" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26" t="s">
-        <v>91</v>
-      </c>
-      <c r="D26" t="s">
-        <v>80</v>
-      </c>
-      <c r="E26" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>14</v>
-      </c>
-      <c r="B27" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" t="s">
-        <v>40</v>
-      </c>
-      <c r="E27" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>21</v>
-      </c>
-      <c r="B28" t="s">
-        <v>59</v>
-      </c>
-      <c r="C28" t="s">
-        <v>60</v>
-      </c>
-      <c r="D28" t="s">
-        <v>61</v>
-      </c>
-      <c r="E28" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>64</v>
-      </c>
-      <c r="B29" t="s">
-        <v>75</v>
-      </c>
-      <c r="C29" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>65</v>
-      </c>
-      <c r="B30" t="s">
-        <v>76</v>
-      </c>
-      <c r="C30" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>24</v>
-      </c>
-      <c r="B31" t="s">
-        <v>65</v>
-      </c>
-      <c r="C31" t="s">
-        <v>92</v>
-      </c>
-      <c r="D31" t="s">
-        <v>93</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>36</v>
-      </c>
-      <c r="B32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C32" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>20</v>
-      </c>
-      <c r="B33" t="s">
-        <v>58</v>
-      </c>
-      <c r="C33" t="s">
-        <v>55</v>
-      </c>
-      <c r="D33" t="s">
-        <v>56</v>
-      </c>
-      <c r="E33" t="s">
-        <v>57</v>
-      </c>
-      <c r="F33" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>19</v>
-      </c>
-      <c r="B34" t="s">
-        <v>54</v>
-      </c>
-      <c r="C34" t="s">
-        <v>55</v>
-      </c>
-      <c r="D34" t="s">
-        <v>56</v>
-      </c>
-      <c r="E34" t="s">
-        <v>57</v>
-      </c>
-      <c r="F34" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>12</v>
-      </c>
-      <c r="B35" t="s">
-        <v>30</v>
-      </c>
-      <c r="C35" t="s">
-        <v>31</v>
-      </c>
-      <c r="D35" t="s">
-        <v>32</v>
-      </c>
-      <c r="E35" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>13</v>
-      </c>
-      <c r="B36" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36" t="s">
-        <v>35</v>
-      </c>
-      <c r="D36" t="s">
-        <v>36</v>
-      </c>
-      <c r="E36" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>66</v>
-      </c>
-      <c r="B37" t="s">
-        <v>77</v>
-      </c>
-      <c r="C37" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>1</v>
-      </c>
-      <c r="B38" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" t="s">
-        <v>7</v>
-      </c>
-      <c r="E38" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>23</v>
-      </c>
-      <c r="B39" t="s">
-        <v>64</v>
-      </c>
-      <c r="C39" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>15</v>
-      </c>
-      <c r="B40" t="s">
-        <v>42</v>
-      </c>
-      <c r="C40" t="s">
-        <v>43</v>
-      </c>
-      <c r="D40" t="s">
-        <v>44</v>
-      </c>
-      <c r="E40" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>40</v>
-      </c>
-      <c r="C41" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>103</v>
-      </c>
-      <c r="E42" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>102</v>
-      </c>
-      <c r="E43" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>105</v>
-      </c>
-      <c r="C44" t="s">
-        <v>108</v>
-      </c>
-      <c r="D44" t="s">
-        <v>107</v>
-      </c>
-      <c r="E44" t="s">
-        <v>106</v>
-      </c>
+      <c r="E44" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F44" s="1"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F41">
-    <sortCondition ref="B2:B41"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F44">
+    <sortCondition ref="A2:A44"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="E31" r:id="rId1" xr:uid="{09D5DDD7-C332-4C3A-A414-8BA49F0159A2}"/>
-    <hyperlink ref="E8" r:id="rId2" xr:uid="{8B8A37D2-C47D-4C10-8C78-CE8D2C01A8F0}"/>
-    <hyperlink ref="E9" r:id="rId3" display="https://the-mas.org/wp-content/uploads/2018/11/emmff_ascii.txt" xr:uid="{99D944A6-5E59-4D67-B508-62EA24DF2501}"/>
-    <hyperlink ref="E22" r:id="rId4" display="https://the-mas.org/wp-content/uploads/2018/11/emmff_ascii.txt" xr:uid="{FF5495F2-692C-4B33-8927-1A72BE073684}"/>
-    <hyperlink ref="E3" r:id="rId5" xr:uid="{66901B56-F6D0-44E9-903D-BDD45AA319BF}"/>
-    <hyperlink ref="E20" r:id="rId6" xr:uid="{EC2825FC-C6BE-4F83-B527-7C920BF97845}"/>
+    <hyperlink ref="E25" r:id="rId1" xr:uid="{09D5DDD7-C332-4C3A-A414-8BA49F0159A2}"/>
+    <hyperlink ref="E26" r:id="rId2" xr:uid="{8B8A37D2-C47D-4C10-8C78-CE8D2C01A8F0}"/>
+    <hyperlink ref="E40" r:id="rId3" display="https://the-mas.org/wp-content/uploads/2018/11/emmff_ascii.txt" xr:uid="{99D944A6-5E59-4D67-B508-62EA24DF2501}"/>
+    <hyperlink ref="E44" r:id="rId4" display="https://the-mas.org/wp-content/uploads/2018/11/emmff_ascii.txt" xr:uid="{FF5495F2-692C-4B33-8927-1A72BE073684}"/>
+    <hyperlink ref="E39" r:id="rId5" xr:uid="{66901B56-F6D0-44E9-903D-BDD45AA319BF}"/>
+    <hyperlink ref="E31" r:id="rId6" xr:uid="{EC2825FC-C6BE-4F83-B527-7C920BF97845}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>

</xml_diff>

<commit_message>
code and test for generating schema.org and PDS labels from ADA database
</commit_message>
<xml_diff>
--- a/ADA-FileExtensions.xlsx
+++ b/ADA-FileExtensions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944a82e2ddcde9eb/Documents/GithubC/smrgeoinfo/ada-metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{CD0A3E6C-559D-445F-B1A2-7F3E2CEF4369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5278F8FD-E7D9-45C8-852C-228527120FB1}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{CD0A3E6C-559D-445F-B1A2-7F3E2CEF4369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AAC8AAD-1904-425C-8753-7F2177194A09}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="25965" windowHeight="14010" xr2:uid="{6B927432-2DD4-440C-AC82-B9813562449D}"/>
+    <workbookView xWindow="2220" yWindow="3270" windowWidth="25965" windowHeight="14010" xr2:uid="{6B927432-2DD4-440C-AC82-B9813562449D}"/>
   </bookViews>
   <sheets>
     <sheet name="adaFileExtensions" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="142">
   <si>
     <t>id</t>
   </si>
@@ -413,9 +413,6 @@
     <t>application/x-cpg</t>
   </si>
   <si>
-    <t>extension used for text and binary files, need to know the context to get the type either text/plain or application/octet-stream</t>
-  </si>
-  <si>
     <t>application/x-dbf</t>
   </si>
   <si>
@@ -456,6 +453,12 @@
   </si>
   <si>
     <t xml:space="preserve"> HDF5-based interchange file format for electron microscopy data and metadata; h5 dump will work with example I have</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apparently not instances </t>
+  </si>
+  <si>
+    <t>extension used for text and binary files, need to know the context to get the type either text/plain or application/octet-stream.  Instances are tabular data type Electron microprobe analysis</t>
   </si>
 </sst>
 </file>
@@ -1338,8 +1341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D95B8BC-088D-4878-B6B7-898DD2B70A3D}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1585,7 +1588,9 @@
       <c r="E13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -1824,7 +1829,7 @@
         <v>96</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1926,7 +1931,7 @@
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1945,7 +1950,7 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>62</v>
       </c>
@@ -1960,7 +1965,7 @@
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1974,11 +1979,11 @@
         <v>82</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1992,11 +1997,11 @@
         <v>83</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2010,7 +2015,7 @@
         <v>84</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -2026,7 +2031,7 @@
         <v>85</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -2077,16 +2082,16 @@
         <v>102</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="275.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2115,7 +2120,7 @@
         <v>101</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>36</v>
@@ -2124,7 +2129,7 @@
         <v>103</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="60" x14ac:dyDescent="0.25">

</xml_diff>